<commit_message>
Data update day 10/08/2024
</commit_message>
<xml_diff>
--- a/Draft/url_fake.xlsx
+++ b/Draft/url_fake.xlsx
@@ -27,268 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/529056813009174?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/529222722992583?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/529258009655721?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/pfbid0Fyqv6ieJvF2idEP6EjWC8Y56NpZkiq1vkPs1mgRNuRXwGqc83FPe6zywuQuo8PrHl</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/529290529652469?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/529320552982800?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/528811429700379?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/528768566371332?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/528717349709787?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/528628076385381?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/528552849726237?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/528487339732788?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/528159986432190?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/528128189768703?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/528062526441936?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/528038056444383?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/527981793116676?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/527910876457101?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/527939126454276?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/527842579797264?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/527489799832542?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/527437756504413?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/527412146506974?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/527371869844335?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/527252576522931?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/527206429860879?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/527179266530262?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/526908316557357?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/526889329892589?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/526858829895639?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/526818929899629?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/526642786583910?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/526606726587516?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/526256669955855?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/526228633291992?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/526162769965245?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/526001249981397?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/525978446650344?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/525959413318914?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/525927433322112?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/525615780019944?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/525594380022084?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/525321776716011?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/525369186711270?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/525560370025485?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/525284716719717?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/525030856745103?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/524935066754682?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/524791476769041?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/524677946780394?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/524654940116028?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/524341176814071?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/523725196875669?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/523609800220542?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/522905853624270?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/523529200228602?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/522301217018067?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/521903460391176?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/521249890456533?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/521213320460190?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/521106473804208?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/521047017143487?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/520998910481631?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/520964883818367?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/520675637180625?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/520646373850218?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/520623373852518?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/520543343860521?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/520029333911922?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/519892533925602?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/519434743971381?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/519335380647984?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/518692170712305?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/518127384102117?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/516317190949803?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/516220470959475?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/515582377689951?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/515046087743580?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/514464507801738?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/514386594476196?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/513964127851776?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/513866507861538?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/513797644535091?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/513193671262155?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/512733497974839?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/512578807990308?ref=embed_post</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/tintuc247247/posts/512302214684634?ref=embed_post</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>https://www.facebook.com/tintuc247247/posts/512134804701375?ref=embed_post</t>
   </si>
@@ -927,11 +666,8 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1467,10 +1203,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A2:A96"/>
+  <dimension ref="A2:A9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="A96" sqref="A96"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
@@ -1515,445 +1251,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1">
-      <c r="A26" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1">
-      <c r="A27" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1">
-      <c r="A28" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1">
-      <c r="A29" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1">
-      <c r="A30" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1">
-      <c r="A31" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1">
-      <c r="A32" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1">
-      <c r="A35" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1">
-      <c r="A37" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1">
-      <c r="A38" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1">
-      <c r="A39" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1">
-      <c r="A40" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1">
-      <c r="A41" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1">
-      <c r="A42" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1">
-      <c r="A43" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1">
-      <c r="A44" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1">
-      <c r="A45" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1">
-      <c r="A46" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1">
-      <c r="A47" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1">
-      <c r="A48" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1">
-      <c r="A49" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1">
-      <c r="A50" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1">
-      <c r="A51" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1">
-      <c r="A52" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1">
-      <c r="A53" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1">
-      <c r="A54" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1">
-      <c r="A55" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1">
-      <c r="A56" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1">
-      <c r="A57" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1">
-      <c r="A58" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1">
-      <c r="A59" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1">
-      <c r="A60" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1">
-      <c r="A61" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1">
-      <c r="A62" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1">
-      <c r="A63" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1">
-      <c r="A64" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1">
-      <c r="A65" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1">
-      <c r="A66" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1">
-      <c r="A67" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1">
-      <c r="A68" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1">
-      <c r="A69" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1">
-      <c r="A70" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1">
-      <c r="A71" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1">
-      <c r="A72" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1">
-      <c r="A73" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1">
-      <c r="A74" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1">
-      <c r="A75" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1">
-      <c r="A76" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1">
-      <c r="A77" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1">
-      <c r="A78" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1">
-      <c r="A79" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1">
-      <c r="A80" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1">
-      <c r="A81" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1">
-      <c r="A82" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1">
-      <c r="A83" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1">
-      <c r="A84" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1">
-      <c r="A85" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1">
-      <c r="A86" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1">
-      <c r="A87" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1">
-      <c r="A88" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1">
-      <c r="A89" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1">
-      <c r="A90" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1">
-      <c r="A91" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1">
-      <c r="A92" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1">
-      <c r="A93" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1">
-      <c r="A94" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1">
-      <c r="A95" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1">
-      <c r="A96" t="s">
-        <v>94</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A76" r:id="rId1" display="https://www.facebook.com/tintuc247247/posts/516317190949803?ref=embed_post"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>